<commit_message>
Ajout de la fonctionnalité GANTT
</commit_message>
<xml_diff>
--- a/Modele_Liste_Tache.xlsx
+++ b/Modele_Liste_Tache.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faustin/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faustin/WebstormProjects/cytoscape.js-klay/vite-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A529BC-CDE3-D040-993A-E1F180932360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3227A5B8-13F7-B344-9AE7-ED3C64834D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15720" xr2:uid="{4C8B706E-9B02-4A7F-9735-6CDFCC829B56}"/>
   </bookViews>
@@ -493,7 +493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -545,7 +545,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -863,7 +862,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -871,7 +870,8 @@
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45" customWidth="1"/>
     <col min="4" max="4" width="17.1640625" customWidth="1"/>
-    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="60.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -933,7 +933,7 @@
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
       <c r="H3" s="5"/>
-      <c r="J3" s="31" t="s">
+      <c r="J3" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>